<commit_message>
modif jeu de données
</commit_message>
<xml_diff>
--- a/Database/Jeu de données.xlsx
+++ b/Database/Jeu de données.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="utilisateur" sheetId="15" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>id_Commentaire</t>
   </si>
@@ -191,6 +191,27 @@
   </si>
   <si>
     <t>Bonjour j'ai un problème.</t>
+  </si>
+  <si>
+    <t>M1102</t>
+  </si>
+  <si>
+    <t>document installation linux</t>
+  </si>
+  <si>
+    <t>correction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on fais comme ca </t>
+  </si>
+  <si>
+    <t>29/10/2016 14:00:00</t>
+  </si>
+  <si>
+    <t>Base d'un système</t>
+  </si>
+  <si>
+    <t>Gestion d'un système</t>
   </si>
 </sst>
 </file>
@@ -214,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +260,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8E5F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -252,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -264,10 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -604,25 +628,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="7.25" customWidth="1"/>
+    <col min="7" max="7" width="5.5" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="16.625" customWidth="1"/>
+    <col min="10" max="10" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -654,37 +676,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>31270</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>781734740</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -709,17 +730,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -727,15 +746,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
@@ -752,20 +771,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="8.25" customWidth="1"/>
+    <col min="4" max="4" width="31.75" customWidth="1"/>
+    <col min="5" max="5" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -782,24 +799,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -819,21 +836,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="B1:C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="20.125" customWidth="1"/>
+    <col min="6" max="6" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -853,27 +868,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -897,7 +912,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -905,20 +920,20 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -935,12 +950,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
@@ -953,23 +985,23 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -977,33 +1009,56 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
@@ -1016,20 +1071,18 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1040,10 +1093,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
@@ -1058,20 +1122,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1088,24 +1150,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>31100</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1126,16 +1188,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1143,15 +1205,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
@@ -1168,18 +1230,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -1190,18 +1250,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1217,20 +1277,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -1238,24 +1297,73 @@
         <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
@@ -1270,18 +1378,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
+    <col min="3" max="3" width="6.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1292,18 +1398,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1319,22 +1425,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1351,29 +1457,46 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
@@ -1386,21 +1509,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="4" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1414,25 +1537,39 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
@@ -1447,18 +1584,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" customWidth="1"/>
+    <col min="2" max="2" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="14.25" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1472,21 +1608,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>

</xml_diff>